<commit_message>
Updated the ESR locators
</commit_message>
<xml_diff>
--- a/data/ESRReport.xlsx
+++ b/data/ESRReport.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abinaya\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{0BE1D138-4292-4416-9BAB-7473F7D9CAD0}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A492760A-495E-49B8-A129-6E5088C6DDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ESR" r:id="rId1" sheetId="1"/>
+    <sheet name="ESR" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,9 +42,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>wakram@dacgroup.com</t>
-  </si>
-  <si>
     <t>Scenario2</t>
   </si>
   <si>
@@ -61,13 +58,15 @@
   </si>
   <si>
     <t>No Email</t>
+  </si>
+  <si>
+    <t>adevaraj@dacgroup.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,19 +102,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -132,10 +131,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -170,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -205,7 +204,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -299,21 +298,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -330,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -382,24 +381,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -421,49 +420,50 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2" xr:uid="{65330ED5-CAA7-4B0A-B07E-8818DAAD59F2}"/>
-    <hyperlink r:id="rId2" ref="C5" xr:uid="{7A900074-2DB8-438F-8DA9-1F584BDA222D}"/>
-    <hyperlink r:id="rId3" ref="C3" xr:uid="{6C3A02BD-9872-4C82-8212-EBF9CBDDB54D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{65330ED5-CAA7-4B0A-B07E-8818DAAD59F2}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{7A900074-2DB8-438F-8DA9-1F584BDA222D}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{6C3A02BD-9872-4C82-8212-EBF9CBDDB54D}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{A2987009-77DB-463D-8255-37B6D0715890}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId4" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the setcellvalue method
</commit_message>
<xml_diff>
--- a/data/ESRReport.xlsx
+++ b/data/ESRReport.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abinaya\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A492760A-495E-49B8-A129-6E5088C6DDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A492760A-495E-49B8-A129-6E5088C6DDC4}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="ESR" sheetId="1" r:id="rId1"/>
+    <sheet name="ESR" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -67,6 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,19 +103,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -131,10 +132,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -169,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -204,7 +205,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -298,21 +299,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -329,7 +330,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -381,15 +382,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -397,8 +398,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,12 +459,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{65330ED5-CAA7-4B0A-B07E-8818DAAD59F2}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{7A900074-2DB8-438F-8DA9-1F584BDA222D}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{6C3A02BD-9872-4C82-8212-EBF9CBDDB54D}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{A2987009-77DB-463D-8255-37B6D0715890}"/>
+    <hyperlink r:id="rId1" ref="C2" xr:uid="{65330ED5-CAA7-4B0A-B07E-8818DAAD59F2}"/>
+    <hyperlink r:id="rId2" ref="C5" xr:uid="{7A900074-2DB8-438F-8DA9-1F584BDA222D}"/>
+    <hyperlink r:id="rId3" ref="C3" xr:uid="{6C3A02BD-9872-4C82-8212-EBF9CBDDB54D}"/>
+    <hyperlink r:id="rId4" ref="C4" xr:uid="{A2987009-77DB-463D-8255-37B6D0715890}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId5" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>